<commit_message>
Folder Structure and Doc Prep
Added orientation pics
Added new print parts
Cleaned up folders
Prepping to create Wiki
</commit_message>
<xml_diff>
--- a/Documentation/BOMs/Wilson Thrust BOM v4 No Grip LEDs.xlsx
+++ b/Documentation/BOMs/Wilson Thrust BOM v4 No Grip LEDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahm\Documents\GitHub\WilsonThrust510\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d7a43267b7fa0998/Github Repositories/WilsonThrust510/Documentation/BOMs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D398573-CD64-4424-BA01-434612055BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C99EEBEB-5120-4843-8B17-4416EAFBA3F3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{C99EEBEB-5120-4843-8B17-4416EAFBA3F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Large PCB Parts" sheetId="1" r:id="rId1"/>
@@ -1070,7 +1070,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1096,45 +1096,19 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1146,37 +1120,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1192,15 +1157,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1519,7 +1475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9BCF817-8F85-4AC7-830C-DC635E268E92}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -1559,15 +1515,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -1588,7 +1544,7 @@
       <c r="F3" s="6">
         <v>1.69</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="18" t="s">
         <v>254</v>
       </c>
     </row>
@@ -1599,10 +1555,10 @@
       <c r="B4" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="4" t="s">
         <v>253</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1613,27 +1569,27 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-    </row>
-    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="4" t="s">
         <v>257</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -1644,15 +1600,15 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -1673,18 +1629,18 @@
       <c r="F8" s="7">
         <v>16.100000000000001</v>
       </c>
-      <c r="G8" s="35"/>
+      <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="21" t="s">
         <v>267</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -1707,15 +1663,15 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -1741,13 +1697,13 @@
       <c r="A13" s="3">
         <v>23</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="31" t="s">
+      <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="4" t="s">
         <v>262</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -1818,15 +1774,15 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="21" t="s">
         <v>269</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -1890,12 +1846,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A17:G17"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A5:G5"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A7:G7"/>
     <mergeCell ref="A9:G9"/>
-    <mergeCell ref="A17:G17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{4B6EC774-7ABE-4E09-B4C8-C546D1757ED3}"/>
@@ -2065,9 +2021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D93DF4F7-3EA2-4CC1-B26E-40F3D884DD27}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22:XFD22"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,22 +2038,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>169</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2105,15 +2061,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -2174,18 +2130,18 @@
       <c r="F5" s="7">
         <v>1.2</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -2206,7 +2162,7 @@
       <c r="F7" s="7">
         <v>9.57</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
@@ -2227,18 +2183,18 @@
       <c r="F8" s="6">
         <v>7.89</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+      <c r="A9" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -2259,24 +2215,24 @@
       <c r="F10" s="6">
         <v>1.99</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="17" t="s">
         <v>241</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -2291,19 +2247,19 @@
       <c r="F12" s="7">
         <v>11.89</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D13" s="29" t="s">
+      <c r="D13" s="4" t="s">
         <v>243</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -2312,20 +2268,20 @@
       <c r="F13" s="7">
         <v>10.89</v>
       </c>
-      <c r="G13" s="30" t="s">
+      <c r="G13" s="9" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -2346,18 +2302,18 @@
       <c r="F15" s="6">
         <v>3.17</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" ht="92.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
@@ -2378,7 +2334,7 @@
       <c r="F17" s="6">
         <v>8.69</v>
       </c>
-      <c r="G17" s="38" t="s">
+      <c r="G17" s="23" t="s">
         <v>72</v>
       </c>
     </row>
@@ -2401,7 +2357,7 @@
       <c r="F18" s="6">
         <v>14.62</v>
       </c>
-      <c r="G18" s="38"/>
+      <c r="G18" s="23"/>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -2413,7 +2369,7 @@
       <c r="C19" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2422,7 +2378,7 @@
       <c r="F19" s="6">
         <v>2.08</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="9" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2436,7 +2392,7 @@
       <c r="C20" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="10" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2445,7 +2401,7 @@
       <c r="F20" s="6">
         <v>5.9578800000000003</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="9" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2456,10 +2412,10 @@
       <c r="B21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="4" t="s">
         <v>167</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2468,20 +2424,20 @@
       <c r="F21" s="6">
         <v>5.5</v>
       </c>
-      <c r="G21" s="28" t="s">
+      <c r="G21" s="9" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="37"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -2502,20 +2458,20 @@
       <c r="F23" s="6">
         <v>18.14</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -2536,7 +2492,7 @@
       <c r="F25" s="6">
         <v>3.99</v>
       </c>
-      <c r="G25" s="12"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
@@ -2557,7 +2513,7 @@
       <c r="F26" s="6">
         <v>3.95</v>
       </c>
-      <c r="G26" s="12"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -2578,20 +2534,20 @@
       <c r="F27" s="6">
         <v>5.18</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="9" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -2600,10 +2556,10 @@
       <c r="B29" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="4" t="s">
         <v>237</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="4" t="s">
         <v>236</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -2612,64 +2568,63 @@
       <c r="F29" s="7">
         <v>2.4900000000000002</v>
       </c>
-      <c r="G29" s="29"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="12"/>
+      <c r="G30" s="9"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="12"/>
+      <c r="G31" s="9"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="12"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="12"/>
+      <c r="G33" s="9"/>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="12"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="12"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="12"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="12"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="12"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="12"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="12"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="12"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="12"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="12"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="12"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="12"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="12"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="12"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="12"/>
+      <c r="G48" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2731,22 +2686,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>169</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -2754,15 +2709,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -2783,20 +2738,20 @@
       <c r="F3" s="6">
         <v>0.1</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" ht="89.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -2817,20 +2772,20 @@
       <c r="F5" s="7">
         <v>7.99</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -2851,18 +2806,17 @@
       <c r="F7" s="7">
         <v>15.18</v>
       </c>
-      <c r="G7" s="14"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -2883,20 +2837,20 @@
       <c r="F9" s="6">
         <v>9.98</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -2917,20 +2871,20 @@
       <c r="F11" s="6">
         <v>7.99</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="9" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2951,65 +2905,65 @@
       <c r="F13" s="6">
         <v>10.15</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="9" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-    </row>
-    <row r="15" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="26">
         <v>3</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="28" t="s">
         <v>172</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="29">
         <v>13.49</v>
       </c>
-      <c r="G15" s="43" t="s">
+      <c r="G15" s="30" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="26" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="25" t="s">
+    <row r="16" spans="1:7" s="16" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="26"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="43"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="21" t="s">
         <v>191</v>
       </c>
-      <c r="B17" s="37"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -3030,7 +2984,7 @@
       <c r="F18" s="6">
         <v>7.89</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
@@ -3051,18 +3005,18 @@
       <c r="F19" s="6">
         <v>7.99</v>
       </c>
-      <c r="G19" s="12"/>
+      <c r="G19" s="9"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="21" t="s">
         <v>192</v>
       </c>
-      <c r="B20" s="37"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -3083,7 +3037,7 @@
       <c r="F21" s="6">
         <v>9.99</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="9" t="s">
         <v>196</v>
       </c>
     </row>
@@ -3106,7 +3060,7 @@
       <c r="F22" s="6">
         <v>12.99</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="9" t="s">
         <v>197</v>
       </c>
     </row>
@@ -3129,20 +3083,20 @@
       <c r="F23" s="6">
         <v>6.99</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="9" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="21" t="s">
         <v>202</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
     </row>
     <row r="25" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -3163,20 +3117,20 @@
       <c r="F25" s="6">
         <v>8.99</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="9" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
     </row>
     <row r="27" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
@@ -3197,20 +3151,20 @@
       <c r="F27" s="6">
         <v>1.22</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="G27" s="9" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="21" t="s">
         <v>188</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
@@ -3231,20 +3185,20 @@
       <c r="F29" s="6">
         <v>5.99</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="G29" s="9" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="21" t="s">
         <v>179</v>
       </c>
-      <c r="B30" s="37"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
     </row>
     <row r="31" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -3265,7 +3219,7 @@
       <c r="F31" s="6">
         <v>4.6900000000000004</v>
       </c>
-      <c r="G31" s="44" t="s">
+      <c r="G31" s="24" t="s">
         <v>186</v>
       </c>
     </row>
@@ -3288,18 +3242,18 @@
       <c r="F32" s="6">
         <v>5.16</v>
       </c>
-      <c r="G32" s="45"/>
+      <c r="G32" s="25"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
+      <c r="A33" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="37"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -3314,81 +3268,76 @@
       <c r="E34" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="G34" s="12"/>
+      <c r="G34" s="9"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="12"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="12"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="12"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="12"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="12"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="12"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="12"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="12"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="12"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="12"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="12"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="12"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="12"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="12"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="12"/>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" s="12"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="12"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="12"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="12"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="12"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="12"/>
+      <c r="G55" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="G31:G32"/>
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A24:G24"/>
-    <mergeCell ref="A26:G26"/>
     <mergeCell ref="A33:G33"/>
     <mergeCell ref="A12:G12"/>
     <mergeCell ref="A14:G14"/>
@@ -3405,6 +3354,11 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="A30:G30"/>
+    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="A28:G28"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A24:G24"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E7" r:id="rId1" xr:uid="{EF6854EA-9FC9-4FFA-B284-7464CDC602EE}"/>
@@ -3451,22 +3405,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>42</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -3474,15 +3428,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -3508,7 +3462,7 @@
       <c r="B4" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="3" t="s">
         <v>218</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -3593,7 +3547,7 @@
       <c r="B9" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="4" t="s">
         <v>220</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -3619,7 +3573,7 @@
       <c r="F10" s="7">
         <v>2.8</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
@@ -3637,7 +3591,7 @@
       <c r="F11" s="7">
         <v>14.47</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
@@ -3655,7 +3609,7 @@
       <c r="F12" s="7">
         <v>10.35</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="9"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -3673,18 +3627,18 @@
       <c r="F13" s="7">
         <v>6.17</v>
       </c>
-      <c r="G13" s="12"/>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
@@ -3705,7 +3659,7 @@
       <c r="F15" s="7">
         <v>15.04</v>
       </c>
-      <c r="G15" s="12"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
@@ -3726,19 +3680,19 @@
       <c r="F16" s="7">
         <v>14.71</v>
       </c>
-      <c r="G16" s="12"/>
+      <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>7</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="4" t="s">
         <v>133</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -3747,7 +3701,7 @@
       <c r="F17" s="6">
         <v>13.69</v>
       </c>
-      <c r="G17" s="30"/>
+      <c r="G17" s="9"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -3768,92 +3722,92 @@
       <c r="F18" s="6">
         <v>12.19</v>
       </c>
-      <c r="G18" s="12"/>
+      <c r="G18" s="9"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-    </row>
-    <row r="20" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>1</v>
-      </c>
-      <c r="B20" s="18" t="s">
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="12">
+        <v>1</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C20" s="21" t="s">
+      <c r="C20" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D20" s="18"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F20" s="22">
+      <c r="F20" s="6">
         <v>6.14</v>
       </c>
-      <c r="G20" s="18"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="21" t="s">
         <v>224</v>
       </c>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-    </row>
-    <row r="22" spans="1:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
-        <v>1</v>
-      </c>
-      <c r="B22" s="18" t="s">
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+    </row>
+    <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C22" s="21" t="s">
+      <c r="C22" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="D22" s="32" t="s">
+      <c r="D22" s="4" t="s">
         <v>226</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="6">
         <v>3.58</v>
       </c>
-      <c r="G22" s="46" t="s">
+      <c r="G22" s="20" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
-        <v>1</v>
-      </c>
-      <c r="B23" s="18" t="s">
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C23" s="21" t="s">
+      <c r="C23" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D23" s="32" t="s">
+      <c r="D23" s="4" t="s">
         <v>271</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="22">
+      <c r="F23" s="6">
         <v>5.49</v>
       </c>
-      <c r="G23" s="46" t="s">
+      <c r="G23" s="20" t="s">
         <v>275</v>
       </c>
     </row>
@@ -3861,13 +3815,13 @@
       <c r="A24" s="3">
         <v>1</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="17" t="s">
         <v>229</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="4" t="s">
         <v>227</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -3876,144 +3830,144 @@
       <c r="F24" s="6">
         <v>4.99</v>
       </c>
-      <c r="G24" s="12"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E25" s="5"/>
-      <c r="G25" s="38"/>
+      <c r="G25" s="23"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E26" s="5"/>
-      <c r="G26" s="38"/>
+      <c r="G26" s="23"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="13"/>
+      <c r="D27" s="10"/>
       <c r="E27" s="5"/>
-      <c r="G27" s="12"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="13"/>
+      <c r="D28" s="10"/>
       <c r="E28" s="5"/>
-      <c r="G28" s="12"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E29" s="5"/>
-      <c r="G29" s="12"/>
-    </row>
-    <row r="30" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="16"/>
+      <c r="G29" s="9"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E31" s="5"/>
-      <c r="G31" s="12"/>
-    </row>
-    <row r="32" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="16"/>
+      <c r="G31" s="9"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E33" s="5"/>
-      <c r="G33" s="12"/>
-    </row>
-    <row r="34" spans="1:7" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="16"/>
+      <c r="G33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="E35" s="5"/>
-      <c r="G35" s="12"/>
+      <c r="G35" s="9"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E36" s="5"/>
-      <c r="G36" s="12"/>
+      <c r="G36" s="9"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E37" s="5"/>
-      <c r="G37" s="12"/>
+      <c r="G37" s="9"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E38" s="5"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="9"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="12"/>
+      <c r="G39" s="9"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="12"/>
+      <c r="G40" s="9"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="12"/>
+      <c r="G41" s="9"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="12"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="12"/>
+      <c r="G43" s="9"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="12"/>
+      <c r="G44" s="9"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="12"/>
+      <c r="G45" s="9"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="12"/>
+      <c r="G46" s="9"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="12"/>
+      <c r="G47" s="9"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="12"/>
+      <c r="G48" s="9"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="12"/>
+      <c r="G49" s="9"/>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" s="12"/>
+      <c r="G50" s="9"/>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="12"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G52" s="12"/>
+      <c r="G52" s="9"/>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G53" s="12"/>
+      <c r="G53" s="9"/>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G54" s="12"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G55" s="12"/>
+      <c r="G55" s="9"/>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G56" s="12"/>
+      <c r="G56" s="9"/>
     </row>
     <row r="57" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G57" s="12"/>
+      <c r="G57" s="9"/>
     </row>
     <row r="58" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G58" s="12"/>
+      <c r="G58" s="9"/>
     </row>
     <row r="59" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G59" s="12"/>
+      <c r="G59" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>